<commit_message>
fix: add Presentation task into data
</commit_message>
<xml_diff>
--- a/dashboard/data/xlsx/Tasks.xlsx
+++ b/dashboard/data/xlsx/Tasks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t xml:space="preserve">task</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">Course work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation</t>
   </si>
 </sst>
 </file>
@@ -241,10 +244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,6 +386,14 @@
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>